<commit_message>
code revision part 2
</commit_message>
<xml_diff>
--- a/exampleAdvanced.xlsx
+++ b/exampleAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronste\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0335F18-A35D-4A41-B3D0-6086C312CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD46C6B-74BF-413E-8379-6F81777DAC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>abstract</t>
   </si>
   <si>
-    <t>issueDatepublished</t>
-  </si>
-  <si>
     <t>issueVolume</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>sectionSeq</t>
+  </si>
+  <si>
+    <t>issueDatePublished</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -722,126 +722,126 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="AH1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="AK1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I2" s="5">
         <v>42808</v>
@@ -856,99 +856,99 @@
         <v>2017</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="P2" s="4">
         <v>1</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AB2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="AH2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AI2" s="4">
         <v>2017</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AK2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="5">
         <v>42808</v>
@@ -963,72 +963,72 @@
         <v>2017</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="P3" s="4">
         <v>1</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD3" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="AI3" s="4">
         <v>2017</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AK3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="5">
         <v>42885</v>
@@ -1043,63 +1043,63 @@
         <v>2017</v>
       </c>
       <c r="N4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="P4" s="4">
         <v>3</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AA4" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="AB4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AI4" s="4">
         <v>2017</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AK4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="5">
         <v>42885</v>
@@ -1114,49 +1114,49 @@
         <v>2017</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="P5" s="4">
         <v>2</v>
       </c>
       <c r="Q5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="AB5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI5" s="4">
         <v>2017</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AK5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code revision part 1
</commit_message>
<xml_diff>
--- a/exampleAdvanced.xlsx
+++ b/exampleAdvanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti-jussinygard/Github/tsvConverter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronste\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D041BD2-09FA-DF47-B7D0-74781FC5AA1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0335F18-A35D-4A41-B3D0-6086C312CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28000" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esimerkki" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
   <si>
     <t>prefix</t>
   </si>
@@ -192,9 +192,6 @@
     <t>fileLocale1</t>
   </si>
   <si>
-    <t>seq</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -313,6 +310,12 @@
   </si>
   <si>
     <t>This is a short biography of the author.</t>
+  </si>
+  <si>
+    <t>articleSeq</t>
+  </si>
+  <si>
+    <t>sectionSeq</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +390,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -666,46 +669,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="32" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="33.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="19" style="4" customWidth="1"/>
     <col min="9" max="9" width="23" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" style="4" customWidth="1"/>
     <col min="11" max="11" width="20" style="4" customWidth="1"/>
     <col min="12" max="12" width="15.33203125" style="4" customWidth="1"/>
     <col min="13" max="13" width="19.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="16.83203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="15.5" style="4" customWidth="1"/>
-    <col min="16" max="17" width="8.83203125" style="6"/>
-    <col min="18" max="18" width="24.83203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.5" style="4" customWidth="1"/>
-    <col min="20" max="20" width="21.83203125" style="4" customWidth="1"/>
-    <col min="21" max="22" width="19.6640625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="13.5" style="4" customWidth="1"/>
-    <col min="25" max="25" width="16.33203125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.83203125" style="4"/>
-    <col min="28" max="29" width="12.5" style="4" customWidth="1"/>
-    <col min="30" max="33" width="8.83203125" style="4"/>
-    <col min="34" max="36" width="25.1640625" style="4" customWidth="1"/>
-    <col min="37" max="16384" width="8.83203125" style="4"/>
+    <col min="14" max="14" width="16.77734375" style="4" customWidth="1"/>
+    <col min="15" max="16" width="15.44140625" style="4" customWidth="1"/>
+    <col min="17" max="18" width="8.77734375" style="6"/>
+    <col min="19" max="19" width="24.77734375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="21.44140625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="21.77734375" style="4" customWidth="1"/>
+    <col min="22" max="23" width="19.6640625" style="4" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="13.44140625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="16.33203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="16.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="8.77734375" style="4"/>
+    <col min="29" max="30" width="12.44140625" style="4" customWidth="1"/>
+    <col min="31" max="34" width="8.77734375" style="4"/>
+    <col min="35" max="37" width="25.109375" style="4" customWidth="1"/>
+    <col min="38" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1">
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,16 +722,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -751,71 +754,74 @@
       <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>90</v>
+      <c r="AK1" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -829,10 +835,10 @@
         <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>52</v>
@@ -858,71 +864,74 @@
       <c r="O2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>59</v>
+      <c r="P2" s="4">
+        <v>1</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="R2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="W2" s="4" t="s">
+      <c r="V2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AI2" s="4">
         <v>2017</v>
       </c>
-      <c r="AI2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>91</v>
+      <c r="AJ2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
@@ -933,10 +942,10 @@
         <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>52</v>
@@ -962,58 +971,61 @@
       <c r="O3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>2017</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK3" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>2017</v>
-      </c>
-      <c r="AI3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36">
-      <c r="B4" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>52</v>
@@ -1036,55 +1048,58 @@
       <c r="O4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>58</v>
+      <c r="P4" s="4">
+        <v>3</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Z4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AI4" s="4">
         <v>2017</v>
       </c>
-      <c r="AI4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>91</v>
+      <c r="AJ4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK4" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="5">
         <v>42885</v>
@@ -1104,50 +1119,53 @@
       <c r="O5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AC5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH5" s="4">
+      <c r="AD5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI5" s="4">
         <v>2017</v>
       </c>
-      <c r="AI5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>91</v>
+      <c r="AJ5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK5" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AJ2" r:id="rId1" xr:uid="{AF959766-1FA3-6A46-952C-CB2C5867F149}"/>
-    <hyperlink ref="AJ3" r:id="rId2" xr:uid="{7EB292F9-BBE4-4248-83D1-36143486FACE}"/>
-    <hyperlink ref="AJ4" r:id="rId3" xr:uid="{12731871-39DB-F04C-B653-20688EFFEE0E}"/>
-    <hyperlink ref="AJ5" r:id="rId4" xr:uid="{6367547E-5FD2-B249-AE65-E99E8724C184}"/>
-    <hyperlink ref="U2" r:id="rId5" xr:uid="{B8B02464-9B76-D044-9889-2DB42CFB3D18}"/>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{AF959766-1FA3-6A46-952C-CB2C5867F149}"/>
+    <hyperlink ref="AK3" r:id="rId2" xr:uid="{7EB292F9-BBE4-4248-83D1-36143486FACE}"/>
+    <hyperlink ref="AK4" r:id="rId3" xr:uid="{12731871-39DB-F04C-B653-20688EFFEE0E}"/>
+    <hyperlink ref="AK5" r:id="rId4" xr:uid="{6367547E-5FD2-B249-AE65-E99E8724C184}"/>
+    <hyperlink ref="V2" r:id="rId5" xr:uid="{B8B02464-9B76-D044-9889-2DB42CFB3D18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
added support for cover images
</commit_message>
<xml_diff>
--- a/exampleAdvanced.xlsx
+++ b/exampleAdvanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronste\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38629E93-436F-45DD-B079-947A60CCF905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F6F45-6411-43CA-8BDE-7E612E16588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
   <si>
     <t>title</t>
   </si>
@@ -331,6 +331,36 @@
   </si>
   <si>
     <t>Author</t>
+  </si>
+  <si>
+    <t>articleCoverImage</t>
+  </si>
+  <si>
+    <t>de:articleCoverImage</t>
+  </si>
+  <si>
+    <t>issueCoverImage</t>
+  </si>
+  <si>
+    <t>issueCoverImageAltText</t>
+  </si>
+  <si>
+    <t>de:articleCoverImageAltText</t>
+  </si>
+  <si>
+    <t>ISSUE COVER ALT TEXT</t>
+  </si>
+  <si>
+    <t>issue-cover.png</t>
+  </si>
+  <si>
+    <t>article-cover-en.png</t>
+  </si>
+  <si>
+    <t>article-cover-de.png</t>
+  </si>
+  <si>
+    <t>ARTICLE COVER ALT TEXT DE</t>
   </si>
 </sst>
 </file>
@@ -694,11 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ5"/>
+  <dimension ref="A1:AV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL2" sqref="AL2:AL5"/>
+      <selection pane="bottomLeft" activeCell="AT4" sqref="AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -730,7 +760,7 @@
     <col min="42" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -860,8 +890,23 @@
       <c r="AQ1" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" ht="36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" ht="36" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -986,7 +1031,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
@@ -1068,8 +1113,17 @@
       <c r="AN3" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="AR3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" ht="36" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
@@ -1133,8 +1187,14 @@
       <c r="AL4" s="3">
         <v>2018</v>
       </c>
+      <c r="AU4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" ht="36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:48" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>

</xml_diff>